<commit_message>
subject data with height and weight based on gender
</commit_message>
<xml_diff>
--- a/static/course_data/subjects.xlsx
+++ b/static/course_data/subjects.xlsx
@@ -441,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.4722777238463001</v>
+        <v>0.8491677981605887</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>0.7761547671427564</v>
+        <v>0.7723859632085759</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>0.8521311398164599</v>
+        <v>0.6849686434590107</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <v>0.7795373773096899</v>
+        <v>0.4944097202441572</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -533,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="G6">
-        <v>0.4377720999198036</v>
+        <v>0.4796409715614344</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -556,7 +556,7 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <v>0.7836797033794513</v>
+        <v>0.4182311763765975</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.4520536880073199</v>
+        <v>0.8292091300608783</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -602,7 +602,7 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <v>0.347299867773276</v>
+        <v>0.4149378744645645</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -625,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>0.351527583534658</v>
+        <v>0.3719659903562893</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -648,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="G11">
-        <v>0.6557464376960802</v>
+        <v>0.6152954047992178</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -671,7 +671,7 @@
         <v>3</v>
       </c>
       <c r="G12">
-        <v>0.772724688847597</v>
+        <v>0.6599983927921722</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0.5439999779440052</v>
+        <v>0.7650783312204882</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -717,7 +717,7 @@
         <v>3</v>
       </c>
       <c r="G14">
-        <v>0.4221481356336573</v>
+        <v>0.470489115488017</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -740,7 +740,7 @@
         <v>2</v>
       </c>
       <c r="G15">
-        <v>0.8173519834484563</v>
+        <v>0.7865524780453598</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -763,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="G16">
-        <v>0.3276141946728874</v>
+        <v>0.483924011257387</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -786,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="G17">
-        <v>0.3982149331592433</v>
+        <v>0.5523928978350134</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="G18">
-        <v>0.7795373773096899</v>
+        <v>0.4944097202441572</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -832,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="G19">
-        <v>0.4665678913492643</v>
+        <v>0.4968036142363831</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -855,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.5872082966778365</v>
+        <v>0.907553500123203</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -878,7 +878,7 @@
         <v>4</v>
       </c>
       <c r="G21">
-        <v>0.7795942244167546</v>
+        <v>0.5395888920802145</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -901,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="G22">
-        <v>0.6181100448558602</v>
+        <v>0.3197260294040347</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -924,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0.3822858728062785</v>
+        <v>0.6132652609609879</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -947,7 +947,7 @@
         <v>2</v>
       </c>
       <c r="G24">
-        <v>0.6687027970071611</v>
+        <v>0.7290134954065851</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>0.2958800492147244</v>
+        <v>0.5644038803861399</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -993,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="G26">
-        <v>0.7432814259548653</v>
+        <v>0.4839942998610416</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1016,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>0.3659858070786579</v>
+        <v>0.5819868947169489</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1039,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="G28">
-        <v>0.6543279129364101</v>
+        <v>0.4919632623128883</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1062,7 +1062,7 @@
         <v>5</v>
       </c>
       <c r="G29">
-        <v>0.709076053338385</v>
+        <v>0.3916530952949716</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <v>0.3767462886442774</v>
+        <v>0.6032429704482737</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1108,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="G31">
-        <v>0.3082678123618235</v>
+        <v>0.4593934282058102</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1131,7 +1131,7 @@
         <v>5</v>
       </c>
       <c r="G32">
-        <v>0.9297963236582877</v>
+        <v>0.4609677124567014</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1154,7 +1154,7 @@
         <v>3</v>
       </c>
       <c r="G33">
-        <v>0.2491489022258505</v>
+        <v>0.297258174669975</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1177,7 +1177,7 @@
         <v>2</v>
       </c>
       <c r="G34">
-        <v>0.4388227972604585</v>
+        <v>0.5694724822919107</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1200,7 +1200,7 @@
         <v>5</v>
       </c>
       <c r="G35">
-        <v>0.7930267150276797</v>
+        <v>0.3754192414221778</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1223,7 +1223,7 @@
         <v>2</v>
       </c>
       <c r="G36">
-        <v>0.4822161398022782</v>
+        <v>0.6126308757744025</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1246,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="G37">
-        <v>0.7863508404846586</v>
+        <v>0.7759990689976908</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1269,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="G38">
-        <v>0.3029694589627219</v>
+        <v>0.3709858306935775</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1292,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="G39">
-        <v>0.5051994074515435</v>
+        <v>0.6318362912851561</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1315,7 +1315,7 @@
         <v>4</v>
       </c>
       <c r="G40">
-        <v>0.3768880117333277</v>
+        <v>0.2882116139072844</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1338,7 +1338,7 @@
         <v>5</v>
       </c>
       <c r="G41">
-        <v>0.5377728789159922</v>
+        <v>0.2867827098757236</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <v>0.2583295064198891</v>
+        <v>0.4964384236824252</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1384,7 +1384,7 @@
         <v>3</v>
       </c>
       <c r="G43">
-        <v>0.4299408667766249</v>
+        <v>0.4721599366036439</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1407,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>0.2552785016787867</v>
+        <v>0.6122895312109643</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1430,7 +1430,7 @@
         <v>5</v>
       </c>
       <c r="G45">
-        <v>0.4992067504402891</v>
+        <v>0.2839781140898264</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="G46">
-        <v>0.5215634590035082</v>
+        <v>0.4218153869244965</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1476,7 +1476,7 @@
         <v>5</v>
       </c>
       <c r="G47">
-        <v>0.3442284831113022</v>
+        <v>0.1135279230671618</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1499,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="G48">
-        <v>0.8521311398164599</v>
+        <v>0.6849686434590107</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="G49">
-        <v>0.4238644554840234</v>
+        <v>0.6744829344722404</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1545,7 +1545,7 @@
         <v>3</v>
       </c>
       <c r="G50">
-        <v>0.6755520568150297</v>
+        <v>0.5854401457828373</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1568,7 +1568,7 @@
         <v>4</v>
       </c>
       <c r="G51">
-        <v>0.7915286056948826</v>
+        <v>0.5435231740975025</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1591,7 +1591,7 @@
         <v>4</v>
       </c>
       <c r="G52">
-        <v>0.6055912238475708</v>
+        <v>0.4376931575224037</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1614,7 +1614,7 @@
         <v>5</v>
       </c>
       <c r="G53">
-        <v>0.5294739445961635</v>
+        <v>0.3041568691592294</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <v>0.4583263609469006</v>
+        <v>0.8356084560731012</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1660,7 +1660,7 @@
         <v>2</v>
       </c>
       <c r="G55">
-        <v>0.3634505663736035</v>
+        <v>0.4538697727032857</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1683,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="G56">
-        <v>0.5663176046310514</v>
+        <v>0.7973368571272392</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1706,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="G57">
-        <v>0.6419636369789886</v>
+        <v>0.3284336678310721</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1729,7 +1729,7 @@
         <v>4</v>
       </c>
       <c r="G58">
-        <v>0.7795942244167546</v>
+        <v>0.5395888920802145</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1752,7 +1752,7 @@
         <v>4</v>
       </c>
       <c r="G59">
-        <v>0.3867942996096109</v>
+        <v>0.3236188503050357</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="G60">
-        <v>0.4050359554461264</v>
+        <v>0.6805100198486765</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1798,7 +1798,7 @@
         <v>5</v>
       </c>
       <c r="G61">
-        <v>0.9023637538451655</v>
+        <v>0.4536916633670262</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1821,7 +1821,7 @@
         <v>4</v>
       </c>
       <c r="G62">
-        <v>0.5215634590035082</v>
+        <v>0.4218153869244965</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <v>0.3227371553346751</v>
+        <v>0.7234819039569517</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="G64">
-        <v>0.5180615725640193</v>
+        <v>0.8871683678577154</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1890,7 +1890,7 @@
         <v>2</v>
       </c>
       <c r="G65">
-        <v>0.4857227198224454</v>
+        <v>0.6116507161116905</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1913,7 +1913,7 @@
         <v>5</v>
       </c>
       <c r="G66">
-        <v>0.9436528950758842</v>
+        <v>0.4645323187152355</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1936,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="G67">
-        <v>0.4122282887776589</v>
+        <v>0.2186083981247059</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1959,7 +1959,7 @@
         <v>5</v>
       </c>
       <c r="G68">
-        <v>0.452279789510907</v>
+        <v>0.2433294144429285</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1982,7 +1982,7 @@
         <v>3</v>
       </c>
       <c r="G69">
-        <v>0.4135312636196253</v>
+        <v>0.4648981894271831</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="G70">
-        <v>0.4266409012210355</v>
+        <v>0.696609444642862</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2028,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>0.5320080081078782</v>
+        <v>0.8818933569723455</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2051,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <v>0.6699893114646338</v>
+        <v>0.9750297493331613</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2074,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="G73">
-        <v>0.6865136458719472</v>
+        <v>0.9824068675692353</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2097,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>0.5320080081078782</v>
+        <v>0.8818933569723455</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2120,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="G75">
-        <v>0.3688912189261049</v>
+        <v>0.5270824047398788</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2143,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="G76">
-        <v>0.7077435327578451</v>
+        <v>0.4731536445128324</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2166,7 +2166,7 @@
         <v>5</v>
       </c>
       <c r="G77">
-        <v>0.3822838354099491</v>
+        <v>0.172785741343839</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2189,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="G78">
-        <v>0.5758188530279217</v>
+        <v>0.9258634767994663</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2212,7 +2212,7 @@
         <v>5</v>
       </c>
       <c r="G79">
-        <v>0.7032814147297072</v>
+        <v>0.3490299688653611</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2235,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="G80">
-        <v>0.392871356870211</v>
+        <v>0.5082548087806581</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2258,7 +2258,7 @@
         <v>3</v>
       </c>
       <c r="G81">
-        <v>0.6541875499629092</v>
+        <v>0.5781640966931622</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2281,7 +2281,7 @@
         <v>5</v>
       </c>
       <c r="G82">
-        <v>0.2227060578589692</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2304,7 +2304,7 @@
         <v>4</v>
       </c>
       <c r="G83">
-        <v>0.4664537200613883</v>
+        <v>0.38190656847078</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2327,7 +2327,7 @@
         <v>3</v>
       </c>
       <c r="G84">
-        <v>0.6755520568150297</v>
+        <v>0.5854401457828373</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2350,7 +2350,7 @@
         <v>4</v>
       </c>
       <c r="G85">
-        <v>0.6327825222818484</v>
+        <v>0.4823055005862499</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2373,7 +2373,7 @@
         <v>5</v>
       </c>
       <c r="G86">
-        <v>0.4701119369033608</v>
+        <v>0.2621390322429844</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2396,7 +2396,7 @@
         <v>4</v>
       </c>
       <c r="G87">
-        <v>0.4753490371070594</v>
+        <v>0.3889885662701562</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2419,7 +2419,7 @@
         <v>4</v>
       </c>
       <c r="G88">
-        <v>0.8278576724877229</v>
+        <v>0.5549879406118423</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2442,7 +2442,7 @@
         <v>2</v>
       </c>
       <c r="G89">
-        <v>0.7067587342183763</v>
+        <v>0.7456163500746822</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2465,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="G90">
-        <v>0.3506751903569041</v>
+        <v>0.5465264077265201</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2488,7 +2488,7 @@
         <v>3</v>
       </c>
       <c r="G91">
-        <v>0.7413744970048629</v>
+        <v>0.6061435487258003</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2511,7 +2511,7 @@
         <v>4</v>
       </c>
       <c r="G92">
-        <v>0.5950342198962906</v>
+        <v>0.4335884542162834</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2534,7 +2534,7 @@
         <v>4</v>
       </c>
       <c r="G93">
-        <v>0.328704525728251</v>
+        <v>0.2049169701039049</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2557,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="G94">
-        <v>0.3227371553346751</v>
+        <v>0.7234819039569517</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2580,7 +2580,7 @@
         <v>5</v>
       </c>
       <c r="G95">
-        <v>0.5489425156655141</v>
+        <v>0.2917465773713965</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2603,7 +2603,7 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <v>0.3486200247777719</v>
+        <v>0.6638906770639452</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2626,7 +2626,7 @@
         <v>2</v>
       </c>
       <c r="G97">
-        <v>0.3276141946728874</v>
+        <v>0.483924011257387</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2649,7 +2649,7 @@
         <v>4</v>
       </c>
       <c r="G98">
-        <v>0.6388821298988018</v>
+        <v>0.4500469746794989</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2672,7 +2672,7 @@
         <v>3</v>
       </c>
       <c r="G99">
-        <v>0.7076982398295756</v>
+        <v>0.6365514805305428</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2695,7 +2695,7 @@
         <v>5</v>
       </c>
       <c r="G100">
-        <v>0.4070731567989884</v>
+        <v>0.2028812139663073</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2718,7 +2718,7 @@
         <v>3</v>
       </c>
       <c r="G101">
-        <v>0.5617563185221248</v>
+        <v>0.5427036097027333</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="G102">
-        <v>0.5683713989604571</v>
+        <v>0.9213238931118257</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2764,7 +2764,7 @@
         <v>0</v>
       </c>
       <c r="G103">
-        <v>0.3834394859512593</v>
+        <v>0.7855204720290063</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2787,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="G104">
-        <v>0.3840960438689594</v>
+        <v>0.6633712231642477</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2810,7 +2810,7 @@
         <v>4</v>
       </c>
       <c r="G105">
-        <v>0.7098753329289684</v>
+        <v>0.5146744604737933</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2833,7 +2833,7 @@
         <v>4</v>
       </c>
       <c r="G106">
-        <v>0.4609231595769736</v>
+        <v>0.3709543042879361</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2856,7 +2856,7 @@
         <v>5</v>
       </c>
       <c r="G107">
-        <v>0.3834372430995152</v>
+        <v>0.1984296430553029</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2879,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="G108">
-        <v>0.2506940014051346</v>
+        <v>0.601448875862755</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="G109">
-        <v>0.372707730737209</v>
+        <v>0.7182757131413178</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="G110">
-        <v>0.7288150571820369</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2948,7 +2948,7 @@
         <v>1</v>
       </c>
       <c r="G111">
-        <v>0.3840960438689594</v>
+        <v>0.6633712231642477</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2971,7 +2971,7 @@
         <v>5</v>
       </c>
       <c r="G112">
-        <v>0.8093655584495583</v>
+        <v>0.4265305761698831</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2994,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="G113">
-        <v>0.4414037754947052</v>
+        <v>0.7068245185970427</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3017,7 +3017,7 @@
         <v>1</v>
       </c>
       <c r="G114">
-        <v>0.3316810810129083</v>
+        <v>0.6113894539772456</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3040,7 +3040,7 @@
         <v>4</v>
       </c>
       <c r="G115">
-        <v>0.2963242957789028</v>
+        <v>0.2406648854181131</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3063,7 +3063,7 @@
         <v>1</v>
       </c>
       <c r="G116">
-        <v>0.3254968033162551</v>
+        <v>0.6041134048875704</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3086,7 +3086,7 @@
         <v>4</v>
       </c>
       <c r="G117">
-        <v>0.6501500586073572</v>
+        <v>0.4540404210456909</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3109,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="G118">
-        <v>0.3778138574353532</v>
+        <v>0.7279334748679562</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3132,7 +3132,7 @@
         <v>4</v>
       </c>
       <c r="G119">
-        <v>0.4903799392660088</v>
+        <v>0.3867347390390121</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3155,7 +3155,7 @@
         <v>3</v>
       </c>
       <c r="G120">
-        <v>0.5676436923774949</v>
+        <v>0.572137011316726</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3178,7 +3178,7 @@
         <v>5</v>
       </c>
       <c r="G121">
-        <v>0.6299879592372211</v>
+        <v>0.3241155372589398</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3201,7 +3201,7 @@
         <v>2</v>
       </c>
       <c r="G122">
-        <v>0.3579361499266382</v>
+        <v>0.4415159555461904</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3224,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="G123">
-        <v>0.3883005538310135</v>
+        <v>0.7462551651739558</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3247,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="G124">
-        <v>0.5962133936123363</v>
+        <v>0.5873159527665796</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3270,7 +3270,7 @@
         <v>2</v>
       </c>
       <c r="G125">
-        <v>0.8069499064742363</v>
+        <v>0.7830810667970671</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3293,7 +3293,7 @@
         <v>3</v>
       </c>
       <c r="G126">
-        <v>0.3210722443292318</v>
+        <v>0.3099274222842346</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3316,7 +3316,7 @@
         <v>2</v>
       </c>
       <c r="G127">
-        <v>0.5917081415456117</v>
+        <v>0.6640613254063507</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3339,7 +3339,7 @@
         <v>2</v>
       </c>
       <c r="G128">
-        <v>0.3421846660798683</v>
+        <v>0.4005798275755129</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3362,7 +3362,7 @@
         <v>1</v>
       </c>
       <c r="G129">
-        <v>0.5903676110482619</v>
+        <v>0.8116949040162907</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3385,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="G130">
-        <v>0.487009590853711</v>
+        <v>0.520577099532112</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3408,7 +3408,7 @@
         <v>5</v>
       </c>
       <c r="G131">
-        <v>0.9576021543121584</v>
+        <v>0.4680497102560778</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3431,7 +3431,7 @@
         <v>3</v>
       </c>
       <c r="G132">
-        <v>0.4757128164568077</v>
+        <v>0.5017674817320561</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3454,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="G133">
-        <v>0.5321044529633385</v>
+        <v>0.8973834418118962</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3477,7 +3477,7 @@
         <v>5</v>
       </c>
       <c r="G134">
-        <v>0.3665555039703979</v>
+        <v>0.1506429897338237</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3500,7 +3500,7 @@
         <v>4</v>
       </c>
       <c r="G135">
-        <v>0.2532673278475838</v>
+        <v>0.181407067141436</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3523,7 +3523,7 @@
         <v>5</v>
       </c>
       <c r="G136">
-        <v>0.2429313634687682</v>
+        <v>0.04093612797067749</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3546,7 +3546,7 @@
         <v>5</v>
       </c>
       <c r="G137">
-        <v>0.6498232878038794</v>
+        <v>0.367272757893206</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3569,7 +3569,7 @@
         <v>5</v>
       </c>
       <c r="G138">
-        <v>0.8062074934827932</v>
+        <v>0.3789838476807119</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3592,7 +3592,7 @@
         <v>3</v>
       </c>
       <c r="G139">
-        <v>0.5131355717952063</v>
+        <v>0.5207440655363128</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -3615,7 +3615,7 @@
         <v>3</v>
       </c>
       <c r="G140">
-        <v>0.7191493068980754</v>
+        <v>0.599420172424487</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -3638,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="G141">
-        <v>0.402988449303035</v>
+        <v>0.8016198968231919</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3661,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="G142">
-        <v>0.4841596764541625</v>
+        <v>0.8597668468017239</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3684,7 +3684,7 @@
         <v>1</v>
       </c>
       <c r="G143">
-        <v>0.3556648406967512</v>
+        <v>0.5588802248836154</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3707,7 +3707,7 @@
         <v>5</v>
       </c>
       <c r="G144">
-        <v>0.4420929031832289</v>
+        <v>0.237361541294024</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3730,7 +3730,7 @@
         <v>4</v>
       </c>
       <c r="G145">
-        <v>0.4706446990530113</v>
+        <v>0.3763193186558965</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3753,7 +3753,7 @@
         <v>4</v>
       </c>
       <c r="G146">
-        <v>0.864962594770839</v>
+        <v>0.5659781646370312</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3776,7 +3776,7 @@
         <v>1</v>
       </c>
       <c r="G147">
-        <v>0.5193374681582501</v>
+        <v>0.7527245140633929</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3799,7 +3799,7 @@
         <v>5</v>
       </c>
       <c r="G148">
-        <v>0.861926087561127</v>
+        <v>0.4423895671052202</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3822,7 +3822,7 @@
         <v>5</v>
       </c>
       <c r="G149">
-        <v>0.3986545771008683</v>
+        <v>0.1932234522396688</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3845,7 +3845,7 @@
         <v>5</v>
       </c>
       <c r="G150">
-        <v>0.8887890426335308</v>
+        <v>0.4499774884315125</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3868,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="G151">
-        <v>0.3532386587352208</v>
+        <v>0.6756952506354725</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3891,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="G152">
-        <v>0.402988449303035</v>
+        <v>0.8016198968231919</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3914,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="G153">
-        <v>0.2552785016787867</v>
+        <v>0.6122895312109643</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3937,7 +3937,7 @@
         <v>3</v>
       </c>
       <c r="G154">
-        <v>0.7302267349244468</v>
+        <v>0.6028031376506604</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3960,7 +3960,7 @@
         <v>4</v>
       </c>
       <c r="G155">
-        <v>0.4670067505292742</v>
+        <v>0.3743306359396062</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3983,7 +3983,7 @@
         <v>4</v>
       </c>
       <c r="G156">
-        <v>0.267084059673639</v>
+        <v>0.2026631428727608</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -4006,7 +4006,7 @@
         <v>2</v>
       </c>
       <c r="G157">
-        <v>0.7660282929269743</v>
+        <v>0.7687230199080156</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -4029,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="G158">
-        <v>0.4673622390092005</v>
+        <v>0.5990094706308158</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -4052,7 +4052,7 @@
         <v>3</v>
       </c>
       <c r="G159">
-        <v>0.3580332990995145</v>
+        <v>0.3828066457044985</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -4075,7 +4075,7 @@
         <v>3</v>
       </c>
       <c r="G160">
-        <v>0.2251720753685049</v>
+        <v>0.2509570323313369</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -4098,7 +4098,7 @@
         <v>4</v>
       </c>
       <c r="G161">
-        <v>0.4843621814787267</v>
+        <v>0.3958865951124295</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -4121,7 +4121,7 @@
         <v>5</v>
       </c>
       <c r="G162">
-        <v>0.452279789510907</v>
+        <v>0.2433294144429285</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -4144,7 +4144,7 @@
         <v>2</v>
       </c>
       <c r="G163">
-        <v>0.5462828145361674</v>
+        <v>0.6434650243720615</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -4167,7 +4167,7 @@
         <v>5</v>
       </c>
       <c r="G164">
-        <v>0.3514969803135961</v>
+        <v>0.1264845990052011</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -4190,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="G165">
-        <v>0.4640737870974525</v>
+        <v>0.7214461478193539</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -4213,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="G166">
-        <v>0.433695706768307</v>
+        <v>0.8090303749914752</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -4236,7 +4236,7 @@
         <v>4</v>
       </c>
       <c r="G167">
-        <v>0.3695528085617686</v>
+        <v>0.2777961935241688</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -4259,7 +4259,7 @@
         <v>1</v>
       </c>
       <c r="G168">
-        <v>0.3316810810129083</v>
+        <v>0.6113894539772456</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4282,7 +4282,7 @@
         <v>3</v>
       </c>
       <c r="G169">
-        <v>0.4308552407752575</v>
+        <v>0.4759647564682658</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4305,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="G170">
-        <v>0.3312089782154009</v>
+        <v>0.6106007319361725</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -4328,7 +4328,7 @@
         <v>3</v>
       </c>
       <c r="G171">
-        <v>0.2368996653843214</v>
+        <v>0.2751154230599597</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -4351,7 +4351,7 @@
         <v>2</v>
       </c>
       <c r="G172">
-        <v>0.520976868063022</v>
+        <v>0.6439092420184416</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4374,7 +4374,7 @@
         <v>5</v>
       </c>
       <c r="G173">
-        <v>0.6299879592372211</v>
+        <v>0.3241155372589398</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -4397,7 +4397,7 @@
         <v>1</v>
       </c>
       <c r="G174">
-        <v>0.5202140565919037</v>
+        <v>0.7660584908832002</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4420,7 +4420,7 @@
         <v>5</v>
       </c>
       <c r="G175">
-        <v>0.2877890571215618</v>
+        <v>0.1076749812051452</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -4443,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="G176">
-        <v>0.4277329974367512</v>
+        <v>0.801948377192099</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -4466,7 +4466,7 @@
         <v>0</v>
       </c>
       <c r="G177">
-        <v>0.2552785016787867</v>
+        <v>0.6122895312109643</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -4489,7 +4489,7 @@
         <v>3</v>
       </c>
       <c r="G178">
-        <v>0.4619171156560226</v>
+        <v>0.5008970472927593</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -4512,7 +4512,7 @@
         <v>5</v>
       </c>
       <c r="G179">
-        <v>0.5602160597420341</v>
+        <v>0.2966193595707012</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -4535,7 +4535,7 @@
         <v>4</v>
       </c>
       <c r="G180">
-        <v>0.4323548659300354</v>
+        <v>0.3541765670458812</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -4558,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="G181">
-        <v>0.2685651931069038</v>
+        <v>0.5176944994137501</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -4581,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="G182">
-        <v>0.590903384180217</v>
+        <v>0.9347162691951124</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -4604,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="G183">
-        <v>0.4942445512244961</v>
+        <v>0.8619170869901125</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -4627,7 +4627,7 @@
         <v>5</v>
       </c>
       <c r="G184">
-        <v>0.3302347011106426</v>
+        <v>0.08554847103452365</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -4650,7 +4650,7 @@
         <v>2</v>
       </c>
       <c r="G185">
-        <v>0.5112325822750889</v>
+        <v>0.6257545177166426</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -4673,7 +4673,7 @@
         <v>1</v>
       </c>
       <c r="G186">
-        <v>0.6928260530249992</v>
+        <v>0.8624313758265394</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -4696,7 +4696,7 @@
         <v>1</v>
       </c>
       <c r="G187">
-        <v>0.4640737870974525</v>
+        <v>0.7214461478193539</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -4719,7 +4719,7 @@
         <v>0</v>
       </c>
       <c r="G188">
-        <v>0.3522047717467765</v>
+        <v>0.7563087246112919</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -4742,7 +4742,7 @@
         <v>5</v>
       </c>
       <c r="G189">
-        <v>0.295797057842918</v>
+        <v>0.1173327429317836</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -4765,7 +4765,7 @@
         <v>1</v>
       </c>
       <c r="G190">
-        <v>0.5692295654750991</v>
+        <v>0.7768829047920156</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -4788,7 +4788,7 @@
         <v>1</v>
       </c>
       <c r="G191">
-        <v>0.4339868493120823</v>
+        <v>0.7017660955800015</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -4811,7 +4811,7 @@
         <v>0</v>
       </c>
       <c r="G192">
-        <v>0.7202430738026293</v>
+        <v>0.9965733824060192</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -4834,7 +4834,7 @@
         <v>0</v>
       </c>
       <c r="G193">
-        <v>0.3401998072636562</v>
+        <v>0.7436606590263547</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -4857,7 +4857,7 @@
         <v>3</v>
       </c>
       <c r="G194">
-        <v>0.4396516534540901</v>
+        <v>0.4813297708362262</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -4880,7 +4880,7 @@
         <v>5</v>
       </c>
       <c r="G195">
-        <v>0.4893759047343509</v>
+        <v>0.2768961162904502</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -4903,7 +4903,7 @@
         <v>3</v>
       </c>
       <c r="G196">
-        <v>0.3882317527630957</v>
+        <v>0.4473824456546837</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -4926,7 +4926,7 @@
         <v>5</v>
       </c>
       <c r="G197">
-        <v>0.3292476537012631</v>
+        <v>0.1527932299222123</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -4949,7 +4949,7 @@
         <v>3</v>
       </c>
       <c r="G198">
-        <v>0.4396516534540901</v>
+        <v>0.4813297708362262</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -4972,7 +4972,7 @@
         <v>3</v>
       </c>
       <c r="G199">
-        <v>0.7507311614112675</v>
+        <v>0.6524104714658797</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -4995,7 +4995,7 @@
         <v>1</v>
       </c>
       <c r="G200">
-        <v>0.2583295064198891</v>
+        <v>0.4964384236824252</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -5018,7 +5018,7 @@
         <v>2</v>
       </c>
       <c r="G201">
-        <v>0.4527809032219923</v>
+        <v>0.5915989924625322</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -5041,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="G202">
-        <v>0.5985394134431183</v>
+        <v>0.9390343997672448</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -5064,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="G203">
-        <v>0.5953094423709282</v>
+        <v>0.9110249113714955</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -5087,7 +5087,7 @@
         <v>4</v>
       </c>
       <c r="G204">
-        <v>0.8775005390751677</v>
+        <v>0.5695427708955654</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -5110,7 +5110,7 @@
         <v>2</v>
       </c>
       <c r="G205">
-        <v>0.6010026470304904</v>
+        <v>0.6679956074236384</v>
       </c>
     </row>
     <row r="206" spans="1:7">
@@ -5133,7 +5133,7 @@
         <v>5</v>
       </c>
       <c r="G206">
-        <v>0.654036286409853</v>
+        <v>0.3326827053420739</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -5156,7 +5156,7 @@
         <v>2</v>
       </c>
       <c r="G207">
-        <v>0.6409518418490951</v>
+        <v>0.7158425724388069</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
       <c r="G208">
-        <v>0.3486200247777719</v>
+        <v>0.6638906770639452</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -5202,7 +5202,7 @@
         <v>2</v>
       </c>
       <c r="G209">
-        <v>0.6679576560692193</v>
+        <v>0.6940152042217012</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -5225,7 +5225,7 @@
         <v>5</v>
       </c>
       <c r="G210">
-        <v>0.4729937955234972</v>
+        <v>0.2548772850665234</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -5248,7 +5248,7 @@
         <v>4</v>
       </c>
       <c r="G211">
-        <v>0.4230343961215485</v>
+        <v>0.3483398666232583</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -5271,7 +5271,7 @@
         <v>1</v>
       </c>
       <c r="G212">
-        <v>0.4301851735186706</v>
+        <v>0.6821808409643035</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -5294,7 +5294,7 @@
         <v>5</v>
       </c>
       <c r="G213">
-        <v>0.6614553435149679</v>
+        <v>0.3723311809102473</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -5317,7 +5317,7 @@
         <v>3</v>
       </c>
       <c r="G214">
-        <v>0.2195113640556061</v>
+        <v>0.2380003563932978</v>
       </c>
     </row>
     <row r="215" spans="1:7">
@@ -5340,7 +5340,7 @@
         <v>4</v>
       </c>
       <c r="G215">
-        <v>0.360743084175644</v>
+        <v>0.3034400952356326</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -5363,7 +5363,7 @@
         <v>5</v>
       </c>
       <c r="G216">
-        <v>0.654036286409853</v>
+        <v>0.3326827053420739</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -5386,7 +5386,7 @@
         <v>5</v>
       </c>
       <c r="G217">
-        <v>0.8062074934827932</v>
+        <v>0.3789838476807119</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -5409,7 +5409,7 @@
         <v>3</v>
       </c>
       <c r="G218">
-        <v>0.3029694589627219</v>
+        <v>0.3709858306935775</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -5432,7 +5432,7 @@
         <v>0</v>
       </c>
       <c r="G219">
-        <v>0.6865136458719472</v>
+        <v>0.9824068675692353</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="G220">
-        <v>0.448891006914846</v>
+        <v>0.7117883860927156</v>
       </c>
     </row>
     <row r="221" spans="1:7">
@@ -5478,7 +5478,7 @@
         <v>4</v>
       </c>
       <c r="G221">
-        <v>0.6873718568036351</v>
+        <v>0.5058216680781472</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -5501,7 +5501,7 @@
         <v>2</v>
       </c>
       <c r="G222">
-        <v>0.7177517020570972</v>
+        <v>0.7111540009061301</v>
       </c>
     </row>
     <row r="223" spans="1:7">
@@ -5524,7 +5524,7 @@
         <v>1</v>
       </c>
       <c r="G223">
-        <v>0.2485118995081367</v>
+        <v>0.4733317538490918</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -5547,7 +5547,7 @@
         <v>4</v>
       </c>
       <c r="G224">
-        <v>0.6501500586073572</v>
+        <v>0.4540404210456909</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -5570,7 +5570,7 @@
         <v>1</v>
       </c>
       <c r="G225">
-        <v>0.6839195956852872</v>
+        <v>0.8585545306384917</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -5593,7 +5593,7 @@
         <v>0</v>
       </c>
       <c r="G226">
-        <v>0.393678002562833</v>
+        <v>0.7549628036009932</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -5616,7 +5616,7 @@
         <v>2</v>
       </c>
       <c r="G227">
-        <v>0.545305574373077</v>
+        <v>0.6610480387028704</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -5639,7 +5639,7 @@
         <v>3</v>
       </c>
       <c r="G228">
-        <v>0.5617563185221248</v>
+        <v>0.5427036097027333</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -5662,7 +5662,7 @@
         <v>3</v>
       </c>
       <c r="G229">
-        <v>0.3637806745204398</v>
+        <v>0.4286293024853653</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -5685,7 +5685,7 @@
         <v>5</v>
       </c>
       <c r="G230">
-        <v>0.6498232878038794</v>
+        <v>0.367272757893206</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -5708,7 +5708,7 @@
         <v>3</v>
       </c>
       <c r="G231">
-        <v>0.5865995981682524</v>
+        <v>0.5823520852709066</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -5731,7 +5731,7 @@
         <v>5</v>
       </c>
       <c r="G232">
-        <v>0.3986545771008683</v>
+        <v>0.1932234522396688</v>
       </c>
     </row>
     <row r="233" spans="1:7">
@@ -5754,7 +5754,7 @@
         <v>4</v>
       </c>
       <c r="G233">
-        <v>0.5311440268921999</v>
+        <v>0.4279204645088774</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -5777,7 +5777,7 @@
         <v>1</v>
       </c>
       <c r="G234">
-        <v>0.6037296970142751</v>
+        <v>0.791847944354382</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -5800,7 +5800,7 @@
         <v>2</v>
       </c>
       <c r="G235">
-        <v>0.3982149331592433</v>
+        <v>0.5523928978350134</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -5823,7 +5823,7 @@
         <v>2</v>
       </c>
       <c r="G236">
-        <v>0.6388616900092179</v>
+        <v>0.6831745488734919</v>
       </c>
     </row>
     <row r="237" spans="1:7">
@@ -5846,7 +5846,7 @@
         <v>5</v>
       </c>
       <c r="G237">
-        <v>0.5192574192526855</v>
+        <v>0.2975995192334132</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -5869,7 +5869,7 @@
         <v>4</v>
       </c>
       <c r="G238">
-        <v>0.4076274268020021</v>
+        <v>0.3262133564526367</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -5892,7 +5892,7 @@
         <v>2</v>
       </c>
       <c r="G239">
-        <v>0.3210664193810897</v>
+        <v>0.4759962828739072</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -5915,7 +5915,7 @@
         <v>2</v>
       </c>
       <c r="G240">
-        <v>0.4753992228527099</v>
+        <v>0.6056076160315905</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -5938,7 +5938,7 @@
         <v>1</v>
       </c>
       <c r="G241">
-        <v>0.3772675697568303</v>
+        <v>0.6574033500153432</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -5961,7 +5961,7 @@
         <v>1</v>
       </c>
       <c r="G242">
-        <v>0.5692295654750991</v>
+        <v>0.7768829047920156</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -5984,7 +5984,7 @@
         <v>5</v>
       </c>
       <c r="G243">
-        <v>0.6970089989567601</v>
+        <v>0.3869528101325584</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -6007,7 +6007,7 @@
         <v>1</v>
       </c>
       <c r="G244">
-        <v>0.5274944911615818</v>
+        <v>0.7569066348097827</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -6030,7 +6030,7 @@
         <v>4</v>
       </c>
       <c r="G245">
-        <v>0.4404908842387945</v>
+        <v>0.3594515779312512</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -6053,7 +6053,7 @@
         <v>5</v>
       </c>
       <c r="G246">
-        <v>1</v>
+        <v>0.4783307043245247</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -6076,7 +6076,7 @@
         <v>4</v>
       </c>
       <c r="G247">
-        <v>0.9156153728061098</v>
+        <v>0.5799581912786809</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -6099,7 +6099,7 @@
         <v>4</v>
       </c>
       <c r="G248">
-        <v>0.7559923321272771</v>
+        <v>0.5315410283502129</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -6122,7 +6122,7 @@
         <v>2</v>
       </c>
       <c r="G249">
-        <v>0.6777875329134205</v>
+        <v>0.6975325957625436</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -6145,7 +6145,7 @@
         <v>3</v>
       </c>
       <c r="G250">
-        <v>0.5131355717952063</v>
+        <v>0.5207440655363128</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -6168,7 +6168,7 @@
         <v>2</v>
       </c>
       <c r="G251">
-        <v>0.23568916076515</v>
+        <v>0.3150313565409892</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -6191,7 +6191,7 @@
         <v>1</v>
       </c>
       <c r="G252">
-        <v>0.3879290155370771</v>
+        <v>0.6229230226876263</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -6214,7 +6214,7 @@
         <v>3</v>
       </c>
       <c r="G253">
-        <v>0.3853458357120332</v>
+        <v>0.4222209404045851</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -6237,7 +6237,7 @@
         <v>0</v>
       </c>
       <c r="G254">
-        <v>0.393678002562833</v>
+        <v>0.7549628036009932</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -6260,7 +6260,7 @@
         <v>3</v>
       </c>
       <c r="G255">
-        <v>0.2491489022258505</v>
+        <v>0.297258174669975</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -6283,7 +6283,7 @@
         <v>1</v>
       </c>
       <c r="G256">
-        <v>0.5202140565919037</v>
+        <v>0.7660584908832002</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -6306,7 +6306,7 @@
         <v>1</v>
       </c>
       <c r="G257">
-        <v>0.3659858070786579</v>
+        <v>0.5819868947169489</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -6329,7 +6329,7 @@
         <v>1</v>
       </c>
       <c r="G258">
-        <v>0.6403759331782162</v>
+        <v>0.8382729850979166</v>
       </c>
     </row>
     <row r="259" spans="1:7">
@@ -6352,7 +6352,7 @@
         <v>5</v>
       </c>
       <c r="G259">
-        <v>0.8887890426335308</v>
+        <v>0.4499774884315125</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -6375,7 +6375,7 @@
         <v>1</v>
       </c>
       <c r="G260">
-        <v>0.4050359554461264</v>
+        <v>0.6805100198486765</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -6398,7 +6398,7 @@
         <v>0</v>
       </c>
       <c r="G261">
-        <v>0.2951497507566952</v>
+        <v>0.6860171872345667</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -6421,7 +6421,7 @@
         <v>5</v>
       </c>
       <c r="G262">
-        <v>0.7335282047373411</v>
+        <v>0.4008112158978174</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -6444,7 +6444,7 @@
         <v>3</v>
       </c>
       <c r="G263">
-        <v>0.615708469262786</v>
+        <v>0.596973714493218</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6467,7 +6467,7 @@
         <v>0</v>
       </c>
       <c r="G264">
-        <v>0.5475065849431611</v>
+        <v>0.8894812782986378</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -6490,7 +6490,7 @@
         <v>2</v>
       </c>
       <c r="G265">
-        <v>0.5374110142600536</v>
+        <v>0.6391468937999292</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -6513,7 +6513,7 @@
         <v>3</v>
       </c>
       <c r="G266">
-        <v>0.3249987958405112</v>
+        <v>0.3940925005269108</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -6536,7 +6536,7 @@
         <v>2</v>
       </c>
       <c r="G267">
-        <v>0.3807436131395044</v>
+        <v>0.4878170978848284</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -6559,7 +6559,7 @@
         <v>2</v>
       </c>
       <c r="G268">
-        <v>0.5289990707712156</v>
+        <v>0.6497459424410644</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -6582,7 +6582,7 @@
         <v>5</v>
       </c>
       <c r="G269">
-        <v>0.2292741068447889</v>
+        <v>0.0143580468890515</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -6605,7 +6605,7 @@
         <v>2</v>
       </c>
       <c r="G270">
-        <v>0.6409518418490951</v>
+        <v>0.7158425724388069</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -6628,7 +6628,7 @@
         <v>5</v>
       </c>
       <c r="G271">
-        <v>0.3442284831113022</v>
+        <v>0.1135279230671618</v>
       </c>
     </row>
     <row r="272" spans="1:7">
@@ -6651,7 +6651,7 @@
         <v>1</v>
       </c>
       <c r="G272">
-        <v>0.6839195956852872</v>
+        <v>0.8585545306384917</v>
       </c>
     </row>
     <row r="273" spans="1:7">
@@ -6674,7 +6674,7 @@
         <v>3</v>
       </c>
       <c r="G273">
-        <v>0.5218809193200782</v>
+        <v>0.5447354902607345</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -6697,7 +6697,7 @@
         <v>4</v>
       </c>
       <c r="G274">
-        <v>0.4238023051698301</v>
+        <v>0.3433521531370658</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -6720,7 +6720,7 @@
         <v>3</v>
       </c>
       <c r="G275">
-        <v>0.4849428136884348</v>
+        <v>0.5066402639313609</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -6743,7 +6743,7 @@
         <v>1</v>
       </c>
       <c r="G276">
-        <v>0.3840960438689594</v>
+        <v>0.6633712231642477</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -6766,7 +6766,7 @@
         <v>3</v>
       </c>
       <c r="G277">
-        <v>0.6541875499629092</v>
+        <v>0.5781640966931622</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -6789,7 +6789,7 @@
         <v>5</v>
       </c>
       <c r="G278">
-        <v>0.6731976597867596</v>
+        <v>0.3772950484059202</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -6812,7 +6812,7 @@
         <v>1</v>
       </c>
       <c r="G279">
-        <v>0.4121647301958378</v>
+        <v>0.6859856608289252</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -6835,7 +6835,7 @@
         <v>3</v>
       </c>
       <c r="G280">
-        <v>0.5308437243868279</v>
+        <v>0.5504466604617066</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -6858,7 +6858,7 @@
         <v>3</v>
       </c>
       <c r="G281">
-        <v>0.6123468366766438</v>
+        <v>0.5629851552433086</v>
       </c>
     </row>
     <row r="282" spans="1:7">
@@ -6881,7 +6881,7 @@
         <v>5</v>
       </c>
       <c r="G282">
-        <v>0.9857763008626103</v>
+        <v>0.4749477390983511</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -6904,7 +6904,7 @@
         <v>2</v>
       </c>
       <c r="G283">
-        <v>0.6875820944816575</v>
+        <v>0.7374446536639766</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -6927,7 +6927,7 @@
         <v>0</v>
       </c>
       <c r="G284">
-        <v>0.377055950157982</v>
+        <v>0.7799295459681722</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -6950,7 +6950,7 @@
         <v>3</v>
       </c>
       <c r="G285">
-        <v>0.6123468366766438</v>
+        <v>0.5629851552433086</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -6973,7 +6973,7 @@
         <v>4</v>
       </c>
       <c r="G286">
-        <v>0.4804639465353132</v>
+        <v>0.3815780881018727</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -6996,7 +6996,7 @@
         <v>0</v>
       </c>
       <c r="G287">
-        <v>0.3883005538310135</v>
+        <v>0.7462551651739558</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -7019,7 +7019,7 @@
         <v>4</v>
       </c>
       <c r="G288">
-        <v>0.4706446990530113</v>
+        <v>0.3763193186558965</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -7042,7 +7042,7 @@
         <v>5</v>
       </c>
       <c r="G289">
-        <v>0.6063307052186703</v>
+        <v>0.3152627448632938</v>
       </c>
     </row>
     <row r="290" spans="1:7">
@@ -7065,7 +7065,7 @@
         <v>3</v>
       </c>
       <c r="G290">
-        <v>0.4222207243355541</v>
+        <v>0.4644620301115809</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -7088,7 +7088,7 @@
         <v>1</v>
       </c>
       <c r="G291">
-        <v>0.3458029709776526</v>
+        <v>0.5335697317884809</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -7111,7 +7111,7 @@
         <v>5</v>
       </c>
       <c r="G292">
-        <v>0.3903904886333325</v>
+        <v>0.1832011617269546</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -7134,7 +7134,7 @@
         <v>3</v>
       </c>
       <c r="G293">
-        <v>0.7507311614112675</v>
+        <v>0.6524104714658797</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -7157,7 +7157,7 @@
         <v>2</v>
       </c>
       <c r="G294">
-        <v>0.7076647897993745</v>
+        <v>0.7078135898309904</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -7180,7 +7180,7 @@
         <v>1</v>
       </c>
       <c r="G295">
-        <v>0.3879290155370771</v>
+        <v>0.6229230226876263</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -7203,7 +7203,7 @@
         <v>4</v>
       </c>
       <c r="G296">
-        <v>0.6388821298988018</v>
+        <v>0.4500469746794989</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -7226,7 +7226,7 @@
         <v>3</v>
       </c>
       <c r="G297">
-        <v>0.3882317527630957</v>
+        <v>0.4473824456546837</v>
       </c>
     </row>
     <row r="298" spans="1:7">
@@ -7249,7 +7249,7 @@
         <v>5</v>
       </c>
       <c r="G298">
-        <v>0.452279789510907</v>
+        <v>0.2433294144429285</v>
       </c>
     </row>
     <row r="299" spans="1:7">
@@ -7272,7 +7272,7 @@
         <v>5</v>
       </c>
       <c r="G299">
-        <v>0.7930267150276797</v>
+        <v>0.3754192414221778</v>
       </c>
     </row>
     <row r="300" spans="1:7">
@@ -7295,7 +7295,7 @@
         <v>3</v>
       </c>
       <c r="G300">
-        <v>0.8062986109226766</v>
+        <v>0.670988616817361</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -7318,7 +7318,7 @@
         <v>1</v>
       </c>
       <c r="G301">
-        <v>0.3410510842757539</v>
+        <v>0.5199483266448942</v>
       </c>
     </row>
     <row r="302" spans="1:7">
@@ -7341,7 +7341,7 @@
         <v>3</v>
       </c>
       <c r="G302">
-        <v>0.3154190721775862</v>
+        <v>0.2955693753951831</v>
       </c>
     </row>
     <row r="303" spans="1:7">
@@ -7364,7 +7364,7 @@
         <v>0</v>
       </c>
       <c r="G303">
-        <v>0.2462040438371361</v>
+        <v>0.590146779600949</v>
       </c>
     </row>
     <row r="304" spans="1:7">
@@ -7387,7 +7387,7 @@
         <v>4</v>
       </c>
       <c r="G304">
-        <v>0.5120936553297465</v>
+        <v>0.4155666473517822</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -7410,7 +7410,7 @@
         <v>3</v>
       </c>
       <c r="G305">
-        <v>0.4575088372527382</v>
+        <v>0.4917451912193418</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -7433,7 +7433,7 @@
         <v>3</v>
       </c>
       <c r="G306">
-        <v>0.3029694589627219</v>
+        <v>0.3709858306935775</v>
       </c>
     </row>
     <row r="307" spans="1:7">
@@ -7456,7 +7456,7 @@
         <v>1</v>
       </c>
       <c r="G307">
-        <v>0.3506751903569041</v>
+        <v>0.5465264077265201</v>
       </c>
     </row>
     <row r="308" spans="1:7">
@@ -7479,7 +7479,7 @@
         <v>2</v>
       </c>
       <c r="G308">
-        <v>0.8278218275909679</v>
+        <v>0.7899790956393404</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -7502,7 +7502,7 @@
         <v>5</v>
       </c>
       <c r="G309">
-        <v>0.7964724619528998</v>
+        <v>0.4224132971229873</v>
       </c>
     </row>
     <row r="310" spans="1:7">
@@ -7525,7 +7525,7 @@
         <v>4</v>
       </c>
       <c r="G310">
-        <v>0.64350624912584</v>
+        <v>0.4871782827855547</v>
       </c>
     </row>
     <row r="311" spans="1:7">
@@ -7548,7 +7548,7 @@
         <v>0</v>
       </c>
       <c r="G311">
-        <v>0.590903384180217</v>
+        <v>0.9347162691951124</v>
       </c>
     </row>
     <row r="312" spans="1:7">
@@ -7571,7 +7571,7 @@
         <v>5</v>
       </c>
       <c r="G312">
-        <v>0.4893759047343509</v>
+        <v>0.2768961162904502</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -7594,7 +7594,7 @@
         <v>0</v>
       </c>
       <c r="G313">
-        <v>0.3461665583340547</v>
+        <v>0.7500599850385776</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -7617,7 +7617,7 @@
         <v>1</v>
       </c>
       <c r="G314">
-        <v>0.2583295064198891</v>
+        <v>0.4964384236824252</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -7640,7 +7640,7 @@
         <v>0</v>
       </c>
       <c r="G315">
-        <v>0.433695706768307</v>
+        <v>0.8090303749914752</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -7663,7 +7663,7 @@
         <v>2</v>
       </c>
       <c r="G316">
-        <v>0.3748569982653232</v>
+        <v>0.4769764425366191</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -7686,7 +7686,7 @@
         <v>3</v>
       </c>
       <c r="G317">
-        <v>0.5218809193200782</v>
+        <v>0.5447354902607345</v>
       </c>
     </row>
     <row r="318" spans="1:7">
@@ -7709,7 +7709,7 @@
         <v>4</v>
       </c>
       <c r="G318">
-        <v>0.803551065579193</v>
+        <v>0.5474000192855499</v>
       </c>
     </row>
     <row r="319" spans="1:7">
@@ -7732,7 +7732,7 @@
         <v>5</v>
       </c>
       <c r="G319">
-        <v>0.3743377364752278</v>
+        <v>0.1619450859956297</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -7755,7 +7755,7 @@
         <v>3</v>
       </c>
       <c r="G320">
-        <v>0.3268762118533953</v>
+        <v>0.3235488274278214</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -7778,7 +7778,7 @@
         <v>1</v>
       </c>
       <c r="G321">
-        <v>0.5054593219756013</v>
+        <v>0.754756394621394</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -7801,7 +7801,7 @@
         <v>3</v>
       </c>
       <c r="G322">
-        <v>0.5218809193200782</v>
+        <v>0.5447354902607345</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -7824,7 +7824,7 @@
         <v>2</v>
       </c>
       <c r="G323">
-        <v>0.6138977488020155</v>
+        <v>0.7019841666735479</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -7847,7 +7847,7 @@
         <v>0</v>
       </c>
       <c r="G324">
-        <v>0.5464148568699608</v>
+        <v>0.9072200915068738</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -7870,7 +7870,7 @@
         <v>5</v>
       </c>
       <c r="G325">
-        <v>0.8328329705395664</v>
+        <v>0.3859726504698467</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -7893,7 +7893,7 @@
         <v>4</v>
       </c>
       <c r="G326">
-        <v>0.2465690982562823</v>
+        <v>0.1701049708796299</v>
       </c>
     </row>
     <row r="327" spans="1:7">
@@ -7916,7 +7916,7 @@
         <v>2</v>
       </c>
       <c r="G327">
-        <v>0.5552264532064545</v>
+        <v>0.6477140618830632</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -7939,7 +7939,7 @@
         <v>5</v>
       </c>
       <c r="G328">
-        <v>0.2877890571215618</v>
+        <v>0.1076749812051452</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -7962,7 +7962,7 @@
         <v>1</v>
       </c>
       <c r="G329">
-        <v>0.5663176046310514</v>
+        <v>0.7973368571272392</v>
       </c>
     </row>
     <row r="330" spans="1:7">
@@ -7985,7 +7985,7 @@
         <v>4</v>
       </c>
       <c r="G330">
-        <v>0.840140579131042</v>
+        <v>0.558702115547356</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -8008,7 +8008,7 @@
         <v>3</v>
       </c>
       <c r="G331">
-        <v>0.2962009435222202</v>
+        <v>0.3632349486573994</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -8031,7 +8031,7 @@
         <v>1</v>
       </c>
       <c r="G332">
-        <v>0.3443009604788939</v>
+        <v>0.6253694806188953</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -8054,7 +8054,7 @@
         <v>3</v>
       </c>
       <c r="G333">
-        <v>0.8405601725533712</v>
+        <v>0.68154202586503</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -8077,7 +8077,7 @@
         <v>2</v>
       </c>
       <c r="G334">
-        <v>0.5535880289859887</v>
+        <v>0.6665236796831192</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -8100,7 +8100,7 @@
         <v>5</v>
       </c>
       <c r="G335">
-        <v>0.4701119369033608</v>
+        <v>0.2621390322429844</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -8123,7 +8123,7 @@
         <v>2</v>
       </c>
       <c r="G336">
-        <v>0.484016461667469</v>
+        <v>0.6106660390486318</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -8146,7 +8146,7 @@
         <v>1</v>
       </c>
       <c r="G337">
-        <v>0.6403759331782162</v>
+        <v>0.8382729850979166</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -8169,7 +8169,7 @@
         <v>0</v>
       </c>
       <c r="G338">
-        <v>0.6536961056027378</v>
+        <v>0.9674418280068691</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -8192,7 +8192,7 @@
         <v>1</v>
       </c>
       <c r="G339">
-        <v>0.7569596384940596</v>
+        <v>0.8880915189773969</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -8215,7 +8215,7 @@
         <v>0</v>
       </c>
       <c r="G340">
-        <v>0.2599556337188381</v>
+        <v>0.6227049515940799</v>
       </c>
     </row>
     <row r="341" spans="1:7">
@@ -8238,7 +8238,7 @@
         <v>1</v>
       </c>
       <c r="G341">
-        <v>0.6663963946939175</v>
+        <v>0.8161644530864598</v>
       </c>
     </row>
     <row r="342" spans="1:7">
@@ -8261,7 +8261,7 @@
         <v>1</v>
       </c>
       <c r="G342">
-        <v>0.3705162576729277</v>
+        <v>0.6512982724309623</v>
       </c>
     </row>
     <row r="343" spans="1:7">
@@ -8284,7 +8284,7 @@
         <v>4</v>
       </c>
       <c r="G343">
-        <v>0.369316652309247</v>
+        <v>0.310338124077906</v>
       </c>
     </row>
     <row r="344" spans="1:7">
@@ -8307,7 +8307,7 @@
         <v>0</v>
       </c>
       <c r="G344">
-        <v>0.6062372745848981</v>
+        <v>0.9432834372782464</v>
       </c>
     </row>
     <row r="345" spans="1:7">
@@ -8330,7 +8330,7 @@
         <v>0</v>
       </c>
       <c r="G345">
-        <v>0.5464148568699608</v>
+        <v>0.9072200915068738</v>
       </c>
     </row>
     <row r="346" spans="1:7">
@@ -8353,7 +8353,7 @@
         <v>5</v>
       </c>
       <c r="G346">
-        <v>0.4025100292547852</v>
+        <v>0.2120510481988896</v>
       </c>
     </row>
     <row r="347" spans="1:7">
@@ -8376,7 +8376,7 @@
         <v>2</v>
       </c>
       <c r="G347">
-        <v>0.4388227972604585</v>
+        <v>0.5694724822919107</v>
       </c>
     </row>
     <row r="348" spans="1:7">
@@ -8399,7 +8399,7 @@
         <v>3</v>
       </c>
       <c r="G348">
-        <v>0.3799856815626169</v>
+        <v>0.4412773680703026</v>
       </c>
     </row>
     <row r="349" spans="1:7">
@@ -8422,7 +8422,7 @@
         <v>2</v>
       </c>
       <c r="G349">
-        <v>0.5642413578078107</v>
+        <v>0.651896182629453</v>
       </c>
     </row>
     <row r="350" spans="1:7">
@@ -8445,7 +8445,7 @@
         <v>0</v>
       </c>
       <c r="G350">
-        <v>0.6865136458719472</v>
+        <v>0.9824068675692353</v>
       </c>
     </row>
     <row r="351" spans="1:7">
@@ -8468,7 +8468,7 @@
         <v>4</v>
       </c>
       <c r="G351">
-        <v>0.5206991721899131</v>
+        <v>0.401629811751031</v>
       </c>
     </row>
     <row r="352" spans="1:7">
@@ -8491,7 +8491,7 @@
         <v>0</v>
       </c>
       <c r="G352">
-        <v>0.3353969511499904</v>
+        <v>0.624958778825224</v>
       </c>
     </row>
     <row r="353" spans="1:7">
@@ -8514,7 +8514,7 @@
         <v>5</v>
       </c>
       <c r="G353">
-        <v>0.2572554742606581</v>
+        <v>0.06509451869930011</v>
       </c>
     </row>
     <row r="354" spans="1:7">
@@ -8537,7 +8537,7 @@
         <v>3</v>
       </c>
       <c r="G354">
-        <v>0.351527583534658</v>
+        <v>0.3719659903562893</v>
       </c>
     </row>
     <row r="355" spans="1:7">
@@ -8560,7 +8560,7 @@
         <v>3</v>
       </c>
       <c r="G355">
-        <v>0.2819200298445586</v>
+        <v>0.3456753375984429</v>
       </c>
     </row>
     <row r="356" spans="1:7">
@@ -8583,7 +8583,7 @@
         <v>1</v>
       </c>
       <c r="G356">
-        <v>0.3772675697568303</v>
+        <v>0.6574033500153432</v>
       </c>
     </row>
     <row r="357" spans="1:7">
@@ -8606,7 +8606,7 @@
         <v>4</v>
       </c>
       <c r="G357">
-        <v>0.2814429652318715</v>
+        <v>0.2223431951121135</v>
       </c>
     </row>
     <row r="358" spans="1:7">
@@ -8629,7 +8629,7 @@
         <v>5</v>
       </c>
       <c r="G358">
-        <v>0.8328329705395664</v>
+        <v>0.3859726504698467</v>
       </c>
     </row>
     <row r="359" spans="1:7">
@@ -8652,7 +8652,7 @@
         <v>2</v>
       </c>
       <c r="G359">
-        <v>0.7660282929269743</v>
+        <v>0.7687230199080156</v>
       </c>
     </row>
     <row r="360" spans="1:7">
@@ -8675,7 +8675,7 @@
         <v>4</v>
       </c>
       <c r="G360">
-        <v>0.4238023051698301</v>
+        <v>0.3433521531370658</v>
       </c>
     </row>
     <row r="361" spans="1:7">
@@ -8698,7 +8698,7 @@
         <v>1</v>
       </c>
       <c r="G361">
-        <v>0.6914322407378213</v>
+        <v>0.8250164257183787</v>
       </c>
     </row>
     <row r="362" spans="1:7">
@@ -8721,7 +8721,7 @@
         <v>0</v>
       </c>
       <c r="G362">
-        <v>0.2599556337188381</v>
+        <v>0.6227049515940799</v>
       </c>
     </row>
     <row r="363" spans="1:7">
@@ -8744,7 +8744,7 @@
         <v>5</v>
       </c>
       <c r="G363">
-        <v>0.3822838354099491</v>
+        <v>0.172785741343839</v>
       </c>
     </row>
     <row r="364" spans="1:7">
@@ -8767,7 +8767,7 @@
         <v>3</v>
       </c>
       <c r="G364">
-        <v>0.5617563185221248</v>
+        <v>0.5427036097027333</v>
       </c>
     </row>
     <row r="365" spans="1:7">
@@ -8790,7 +8790,7 @@
         <v>0</v>
       </c>
       <c r="G365">
-        <v>0.3532386587352208</v>
+        <v>0.6756952506354725</v>
       </c>
     </row>
     <row r="366" spans="1:7">
@@ -8813,7 +8813,7 @@
         <v>0</v>
       </c>
       <c r="G366">
-        <v>0.5016832208034605</v>
+        <v>0.8660343660370083</v>
       </c>
     </row>
     <row r="367" spans="1:7">
@@ -8836,7 +8836,7 @@
         <v>1</v>
       </c>
       <c r="G367">
-        <v>0.6391884696950993</v>
+        <v>0.8060144591911659</v>
       </c>
     </row>
     <row r="368" spans="1:7">
@@ -8859,7 +8859,7 @@
         <v>2</v>
       </c>
       <c r="G368">
-        <v>0.528611638862644</v>
+        <v>0.6347573859450241</v>
       </c>
     </row>
     <row r="369" spans="1:7">
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="G369">
-        <v>0.2375160314687343</v>
+        <v>0.5659883888723263</v>
       </c>
     </row>
     <row r="370" spans="1:7">
@@ -8905,7 +8905,7 @@
         <v>3</v>
       </c>
       <c r="G370">
-        <v>0.3783290788686547</v>
+        <v>0.4129021183269668</v>
       </c>
     </row>
     <row r="371" spans="1:7">
@@ -8928,7 +8928,7 @@
         <v>3</v>
       </c>
       <c r="G371">
-        <v>0.739852789851107</v>
+        <v>0.6485336262778322</v>
       </c>
     </row>
     <row r="372" spans="1:7">
@@ -8951,7 +8951,7 @@
         <v>2</v>
       </c>
       <c r="G372">
-        <v>0.7966160410669916</v>
+        <v>0.7795636752562248</v>
       </c>
     </row>
     <row r="373" spans="1:7">
@@ -8974,7 +8974,7 @@
         <v>2</v>
       </c>
       <c r="G373">
-        <v>0.4057615641628008</v>
+        <v>0.5583607709839179</v>
       </c>
     </row>
     <row r="374" spans="1:7">
@@ -8997,7 +8997,7 @@
         <v>1</v>
       </c>
       <c r="G374">
-        <v>0.4839244960673041</v>
+        <v>0.7368467434654858</v>
       </c>
     </row>
     <row r="375" spans="1:7">
@@ -9020,7 +9020,7 @@
         <v>4</v>
       </c>
       <c r="G375">
-        <v>0.2336081068316876</v>
+        <v>0.1459465801510073</v>
       </c>
     </row>
     <row r="376" spans="1:7">
@@ -9043,7 +9043,7 @@
         <v>3</v>
       </c>
       <c r="G376">
-        <v>0.7302267349244468</v>
+        <v>0.6028031376506604</v>
       </c>
     </row>
     <row r="377" spans="1:7">
@@ -9066,7 +9066,7 @@
         <v>0</v>
       </c>
       <c r="G377">
-        <v>0.3991428990431568</v>
+        <v>0.7633939618583848</v>
       </c>
     </row>
     <row r="378" spans="1:7">
@@ -9089,7 +9089,7 @@
         <v>1</v>
       </c>
       <c r="G378">
-        <v>0.4365968449275145</v>
+        <v>0.689661875922094</v>
       </c>
     </row>
     <row r="379" spans="1:7">
@@ -9112,7 +9112,7 @@
         <v>2</v>
       </c>
       <c r="G379">
-        <v>0.3690917786281637</v>
+        <v>0.465674346274813</v>
       </c>
     </row>
     <row r="380" spans="1:7">
@@ -9135,7 +9135,7 @@
         <v>0</v>
       </c>
       <c r="G380">
-        <v>0.5872082966778365</v>
+        <v>0.907553500123203</v>
       </c>
     </row>
     <row r="381" spans="1:7">
@@ -9158,7 +9158,7 @@
         <v>4</v>
       </c>
       <c r="G381">
-        <v>0.3484310335449045</v>
+        <v>0.2438488683426262</v>
       </c>
     </row>
     <row r="382" spans="1:7">
@@ -9181,7 +9181,7 @@
         <v>5</v>
       </c>
       <c r="G382">
-        <v>0.4701119369033608</v>
+        <v>0.2621390322429844</v>
       </c>
     </row>
     <row r="383" spans="1:7">
@@ -9204,7 +9204,7 @@
         <v>2</v>
       </c>
       <c r="G383">
-        <v>0.261283997949441</v>
+        <v>0.3801258752402894</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -9227,7 +9227,7 @@
         <v>4</v>
       </c>
       <c r="G384">
-        <v>0.5705492419007013</v>
+        <v>0.4510271343422109</v>
       </c>
     </row>
     <row r="385" spans="1:7">
@@ -9250,7 +9250,7 @@
         <v>4</v>
       </c>
       <c r="G385">
-        <v>0.395695646221109</v>
+        <v>0.3300181763172585</v>
       </c>
     </row>
     <row r="386" spans="1:7">
@@ -9273,7 +9273,7 @@
         <v>3</v>
       </c>
       <c r="G386">
-        <v>0.3328271540415747</v>
+        <v>0.3365055033658606</v>
       </c>
     </row>
     <row r="387" spans="1:7">
@@ -9296,7 +9296,7 @@
         <v>5</v>
       </c>
       <c r="G387">
-        <v>0.3665555039703979</v>
+        <v>0.1506429897338237</v>
       </c>
     </row>
     <row r="388" spans="1:7">
@@ -9319,7 +9319,7 @@
         <v>3</v>
       </c>
       <c r="G388">
-        <v>0.5131355717952063</v>
+        <v>0.5207440655363128</v>
       </c>
     </row>
     <row r="389" spans="1:7">
@@ -9342,7 +9342,7 @@
         <v>4</v>
       </c>
       <c r="G389">
-        <v>0.5104984476756002</v>
+        <v>0.3967570295517263</v>
       </c>
     </row>
     <row r="390" spans="1:7">
@@ -9365,7 +9365,7 @@
         <v>5</v>
       </c>
       <c r="G390">
-        <v>0.9576021543121584</v>
+        <v>0.4680497102560778</v>
       </c>
     </row>
     <row r="391" spans="1:7">
@@ -9388,7 +9388,7 @@
         <v>3</v>
       </c>
       <c r="G391">
-        <v>0.7290541151095492</v>
+        <v>0.6445993442605443</v>
       </c>
     </row>
     <row r="392" spans="1:7">
@@ -9411,7 +9411,7 @@
         <v>5</v>
       </c>
       <c r="G392">
-        <v>0.7799346977062653</v>
+        <v>0.3718061356330629</v>
       </c>
     </row>
     <row r="393" spans="1:7">
@@ -9434,7 +9434,7 @@
         <v>5</v>
       </c>
       <c r="G393">
-        <v>0.5398158338957955</v>
+        <v>0.3105561951714524</v>
       </c>
     </row>
     <row r="394" spans="1:7">
@@ -9457,7 +9457,7 @@
         <v>2</v>
       </c>
       <c r="G394">
-        <v>0.5704069401866542</v>
+        <v>0.6771474634970559</v>
       </c>
     </row>
     <row r="395" spans="1:7">
@@ -9480,7 +9480,7 @@
         <v>4</v>
       </c>
       <c r="G395">
-        <v>0.4576778122705788</v>
+        <v>0.3746305193811047</v>
       </c>
     </row>
     <row r="396" spans="1:7">
@@ -9503,7 +9503,7 @@
         <v>4</v>
       </c>
       <c r="G396">
-        <v>0.6012081193389918</v>
+        <v>0.4671265591363963</v>
       </c>
     </row>
     <row r="397" spans="1:7">
@@ -9526,7 +9526,7 @@
         <v>1</v>
       </c>
       <c r="G397">
-        <v>0.4115012520324471</v>
+        <v>0.6583835096780551</v>
       </c>
     </row>
     <row r="398" spans="1:7">
@@ -9549,7 +9549,7 @@
         <v>1</v>
       </c>
       <c r="G398">
-        <v>0.6750783885818872</v>
+        <v>0.854620248621204</v>
       </c>
     </row>
     <row r="399" spans="1:7">
@@ -9572,7 +9572,7 @@
         <v>1</v>
       </c>
       <c r="G399">
-        <v>0.2633961627962392</v>
+        <v>0.5072790790306344</v>
       </c>
     </row>
     <row r="400" spans="1:7">
@@ -9595,7 +9595,7 @@
         <v>1</v>
       </c>
       <c r="G400">
-        <v>0.5863581418650148</v>
+        <v>0.7844708261183079</v>
       </c>
     </row>
     <row r="401" spans="1:7">
@@ -9618,7 +9618,7 @@
         <v>0</v>
       </c>
       <c r="G401">
-        <v>0.590903384180217</v>
+        <v>0.9347162691951124</v>
       </c>
     </row>
     <row r="402" spans="1:7">
@@ -9641,7 +9641,7 @@
         <v>1</v>
       </c>
       <c r="G402">
-        <v>0.5274944911615818</v>
+        <v>0.7569066348097827</v>
       </c>
     </row>
     <row r="403" spans="1:7">
@@ -9664,7 +9664,7 @@
         <v>2</v>
       </c>
       <c r="G403">
-        <v>0.7067587342183763</v>
+        <v>0.7456163500746822</v>
       </c>
     </row>
     <row r="404" spans="1:7">
@@ -9687,7 +9687,7 @@
         <v>0</v>
       </c>
       <c r="G404">
-        <v>0.5397296199070705</v>
+        <v>0.8857144182763609</v>
       </c>
     </row>
     <row r="405" spans="1:7">
@@ -9710,7 +9710,7 @@
         <v>2</v>
       </c>
       <c r="G405">
-        <v>0.4527809032219923</v>
+        <v>0.5915989924625322</v>
       </c>
     </row>
     <row r="406" spans="1:7">
@@ -9733,7 +9733,7 @@
         <v>1</v>
       </c>
       <c r="G406">
-        <v>0.4301851735186706</v>
+        <v>0.6821808409643035</v>
       </c>
     </row>
     <row r="407" spans="1:7">
@@ -9756,7 +9756,7 @@
         <v>4</v>
       </c>
       <c r="G407">
-        <v>0.5605378649295919</v>
+        <v>0.4454362082813769</v>
       </c>
     </row>
     <row r="408" spans="1:7">
@@ -9779,7 +9779,7 @@
         <v>0</v>
       </c>
       <c r="G408">
-        <v>0.3883005538310135</v>
+        <v>0.7462551651739558</v>
       </c>
     </row>
     <row r="409" spans="1:7">
@@ -9802,7 +9802,7 @@
         <v>4</v>
       </c>
       <c r="G409">
-        <v>0.840140579131042</v>
+        <v>0.558702115547356</v>
       </c>
     </row>
     <row r="410" spans="1:7">
@@ -9825,7 +9825,7 @@
         <v>2</v>
       </c>
       <c r="G410">
-        <v>0.6875820944816575</v>
+        <v>0.7374446536639766</v>
       </c>
     </row>
     <row r="411" spans="1:7">
@@ -9848,7 +9848,7 @@
         <v>2</v>
       </c>
       <c r="G411">
-        <v>0.6388616900092179</v>
+        <v>0.6831745488734919</v>
       </c>
     </row>
     <row r="412" spans="1:7">
@@ -9871,7 +9871,7 @@
         <v>0</v>
       </c>
       <c r="G412">
-        <v>0.5111420658132407</v>
+        <v>0.8819095984117391</v>
       </c>
     </row>
     <row r="413" spans="1:7">
@@ -9894,7 +9894,7 @@
         <v>5</v>
       </c>
       <c r="G413">
-        <v>0.6498232878038794</v>
+        <v>0.367272757893206</v>
       </c>
     </row>
     <row r="414" spans="1:7">
@@ -9917,7 +9917,7 @@
         <v>2</v>
       </c>
       <c r="G414">
-        <v>0.7360713329419118</v>
+        <v>0.7574209236462095</v>
       </c>
     </row>
     <row r="415" spans="1:7">
@@ -9940,7 +9940,7 @@
         <v>5</v>
       </c>
       <c r="G415">
-        <v>0.4122282887776589</v>
+        <v>0.2186083981247059</v>
       </c>
     </row>
     <row r="416" spans="1:7">
@@ -9963,7 +9963,7 @@
         <v>0</v>
       </c>
       <c r="G416">
-        <v>0.6034633651877517</v>
+        <v>0.9144515289654762</v>
       </c>
     </row>
     <row r="417" spans="1:7">
@@ -9986,7 +9986,7 @@
         <v>2</v>
       </c>
       <c r="G417">
-        <v>0.5051994074515435</v>
+        <v>0.6318362912851561</v>
       </c>
     </row>
     <row r="418" spans="1:7">
@@ -10009,7 +10009,7 @@
         <v>4</v>
       </c>
       <c r="G418">
-        <v>0.7443261759827524</v>
+        <v>0.527423749303317</v>
       </c>
     </row>
     <row r="419" spans="1:7">
@@ -10032,7 +10032,7 @@
         <v>3</v>
       </c>
       <c r="G419">
-        <v>0.6123468366766438</v>
+        <v>0.5629851552433086</v>
       </c>
     </row>
     <row r="420" spans="1:7">
@@ -10055,7 +10055,7 @@
         <v>1</v>
       </c>
       <c r="G420">
-        <v>0.5198868720705764</v>
+        <v>0.7530093186121778</v>
       </c>
     </row>
     <row r="421" spans="1:7">
@@ -10078,7 +10078,7 @@
         <v>1</v>
       </c>
       <c r="G421">
-        <v>0.7017972860223557</v>
+        <v>0.8662524371305548</v>
       </c>
     </row>
     <row r="422" spans="1:7">
@@ -10101,7 +10101,7 @@
         <v>3</v>
       </c>
       <c r="G422">
-        <v>0.645607866113331</v>
+        <v>0.6108321202584769</v>
       </c>
     </row>
     <row r="423" spans="1:7">
@@ -10124,7 +10124,7 @@
         <v>3</v>
       </c>
       <c r="G423">
-        <v>0.5717193289167702</v>
+        <v>0.5468857304491231</v>
       </c>
     </row>
     <row r="424" spans="1:7">
@@ -10147,7 +10147,7 @@
         <v>0</v>
       </c>
       <c r="G424">
-        <v>0.2252487635143333</v>
+        <v>0.5250522609016489</v>
       </c>
     </row>
     <row r="425" spans="1:7">
@@ -10170,7 +10170,7 @@
         <v>2</v>
       </c>
       <c r="G425">
-        <v>0.3020201082866799</v>
+        <v>0.4506857897787727</v>
       </c>
     </row>
     <row r="426" spans="1:7">
@@ -10193,7 +10193,7 @@
         <v>4</v>
       </c>
       <c r="G426">
-        <v>0.840140579131042</v>
+        <v>0.558702115547356</v>
       </c>
     </row>
     <row r="427" spans="1:7">
@@ -10216,7 +10216,7 @@
         <v>1</v>
       </c>
       <c r="G427">
-        <v>0.2738346085612974</v>
+        <v>0.5277167899264642</v>
       </c>
     </row>
     <row r="428" spans="1:7">
@@ -10239,7 +10239,7 @@
         <v>3</v>
       </c>
       <c r="G428">
-        <v>0.3249987958405112</v>
+        <v>0.3940925005269108</v>
       </c>
     </row>
     <row r="429" spans="1:7">
@@ -10262,7 +10262,7 @@
         <v>5</v>
       </c>
       <c r="G429">
-        <v>0.2500120143448724</v>
+        <v>0.05328994512777283</v>
       </c>
     </row>
     <row r="430" spans="1:7">
@@ -10285,7 +10285,7 @@
         <v>5</v>
       </c>
       <c r="G430">
-        <v>0.2722167259242589</v>
+        <v>0.08723727030931537</v>
       </c>
     </row>
     <row r="431" spans="1:7">
@@ -10308,7 +10308,7 @@
         <v>3</v>
       </c>
       <c r="G431">
-        <v>0.2251720753685049</v>
+        <v>0.2509570323313369</v>
       </c>
     </row>
     <row r="432" spans="1:7">
@@ -10331,7 +10331,7 @@
         <v>3</v>
       </c>
       <c r="G432">
-        <v>0.5918791759975983</v>
+        <v>0.5550574268598287</v>
       </c>
     </row>
     <row r="433" spans="1:7">
@@ -10354,7 +10354,7 @@
         <v>2</v>
       </c>
       <c r="G433">
-        <v>0.4119164740044874</v>
+        <v>0.5362342608132963</v>
       </c>
     </row>
     <row r="434" spans="1:7">
@@ -10377,7 +10377,7 @@
         <v>5</v>
       </c>
       <c r="G434">
-        <v>0.6850492108281263</v>
+        <v>0.3821678306052249</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -10400,7 +10400,7 @@
         <v>4</v>
       </c>
       <c r="G435">
-        <v>0.815660963455491</v>
+        <v>0.5512210805895654</v>
       </c>
     </row>
     <row r="436" spans="1:7">
@@ -10423,7 +10423,7 @@
         <v>3</v>
       </c>
       <c r="G436">
-        <v>0.5617563185221248</v>
+        <v>0.5427036097027333</v>
       </c>
     </row>
     <row r="437" spans="1:7">
@@ -10446,7 +10446,7 @@
         <v>4</v>
       </c>
       <c r="G437">
-        <v>0.6388821298988018</v>
+        <v>0.4500469746794989</v>
       </c>
     </row>
     <row r="438" spans="1:7">
@@ -10469,7 +10469,7 @@
         <v>1</v>
       </c>
       <c r="G438">
-        <v>0.6403759331782162</v>
+        <v>0.8382729850979166</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -10492,7 +10492,7 @@
         <v>0</v>
       </c>
       <c r="G439">
-        <v>0.4218503305224113</v>
+        <v>0.7946723281024237</v>
       </c>
     </row>
     <row r="440" spans="1:7">
@@ -10515,7 +10515,7 @@
         <v>0</v>
       </c>
       <c r="G440">
-        <v>0.6536961056027378</v>
+        <v>0.9674418280068691</v>
       </c>
     </row>
     <row r="441" spans="1:7">
@@ -10538,7 +10538,7 @@
         <v>1</v>
       </c>
       <c r="G441">
-        <v>0.5523474648406458</v>
+        <v>0.7690717775866802</v>
       </c>
     </row>
     <row r="442" spans="1:7">
@@ -10561,7 +10561,7 @@
         <v>0</v>
       </c>
       <c r="G442">
-        <v>0.3627783739794308</v>
+        <v>0.6978380022454879</v>
       </c>
     </row>
     <row r="443" spans="1:7">
@@ -10584,7 +10584,7 @@
         <v>3</v>
       </c>
       <c r="G443">
-        <v>0.3882317527630957</v>
+        <v>0.4473824456546837</v>
       </c>
     </row>
     <row r="444" spans="1:7">
@@ -10607,7 +10607,7 @@
         <v>5</v>
       </c>
       <c r="G444">
-        <v>0.8354496834194425</v>
+        <v>0.4345784398998848</v>
       </c>
     </row>
     <row r="445" spans="1:7">
@@ -10630,7 +10630,7 @@
         <v>2</v>
       </c>
       <c r="G445">
-        <v>0.5642413578078107</v>
+        <v>0.651896182629453</v>
       </c>
     </row>
     <row r="446" spans="1:7">
@@ -10653,7 +10653,7 @@
         <v>0</v>
       </c>
       <c r="G446">
-        <v>0.4907994857560291</v>
+        <v>0.865478017002696</v>
       </c>
     </row>
     <row r="447" spans="1:7">
@@ -10676,7 +10676,7 @@
         <v>1</v>
       </c>
       <c r="G447">
-        <v>0.3506751903569041</v>
+        <v>0.5465264077265201</v>
       </c>
     </row>
     <row r="448" spans="1:7">
@@ -10699,7 +10699,7 @@
         <v>2</v>
       </c>
       <c r="G448">
-        <v>0.3991079941028397</v>
+        <v>0.5179125705072966</v>
       </c>
     </row>
     <row r="449" spans="1:7">
@@ -10722,7 +10722,7 @@
         <v>1</v>
       </c>
       <c r="G449">
-        <v>0.3379495049892646</v>
+        <v>0.618471451776622</v>
       </c>
     </row>
     <row r="450" spans="1:7">
@@ -10745,7 +10745,7 @@
         <v>3</v>
       </c>
       <c r="G450">
-        <v>0.6557464376960802</v>
+        <v>0.6152954047992178</v>
       </c>
     </row>
     <row r="451" spans="1:7">
@@ -10768,7 +10768,7 @@
         <v>1</v>
       </c>
       <c r="G451">
-        <v>0.2346108643979979</v>
+        <v>0.4343998556103706</v>
       </c>
     </row>
     <row r="452" spans="1:7">
@@ -10791,7 +10791,7 @@
         <v>5</v>
       </c>
       <c r="G452">
-        <v>0.7799346977062653</v>
+        <v>0.3718061356330629</v>
       </c>
     </row>
     <row r="453" spans="1:7">
@@ -10814,7 +10814,7 @@
         <v>3</v>
       </c>
       <c r="G453">
-        <v>0.4537616853743777</v>
+        <v>0.4939990184504859</v>
       </c>
     </row>
     <row r="454" spans="1:7">
@@ -10837,7 +10837,7 @@
         <v>0</v>
       </c>
       <c r="G454">
-        <v>0.3005106157523341</v>
+        <v>0.6939449156180466</v>
       </c>
     </row>
     <row r="455" spans="1:7">
@@ -10860,7 +10860,7 @@
         <v>2</v>
       </c>
       <c r="G455">
-        <v>0.6501256007826026</v>
+        <v>0.7203058569795476</v>
       </c>
     </row>
     <row r="456" spans="1:7">
@@ -10883,7 +10883,7 @@
         <v>4</v>
       </c>
       <c r="G456">
-        <v>0.661502393242323</v>
+        <v>0.4579747030629788</v>
       </c>
     </row>
     <row r="457" spans="1:7">
@@ -10906,7 +10906,7 @@
         <v>5</v>
       </c>
       <c r="G457">
-        <v>0.462580501686049</v>
+        <v>0.2491661148655514</v>
       </c>
     </row>
     <row r="458" spans="1:7">
@@ -10929,7 +10929,7 @@
         <v>2</v>
       </c>
       <c r="G458">
-        <v>0.513043313013967</v>
+        <v>0.637941368869537</v>
       </c>
     </row>
     <row r="459" spans="1:7">
@@ -10952,7 +10952,7 @@
         <v>4</v>
       </c>
       <c r="G459">
-        <v>0.3867942996096109</v>
+        <v>0.3236188503050357</v>
       </c>
     </row>
     <row r="460" spans="1:7">
@@ -10975,7 +10975,7 @@
         <v>0</v>
       </c>
       <c r="G460">
-        <v>0.5397296199070705</v>
+        <v>0.8857144182763609</v>
       </c>
     </row>
     <row r="461" spans="1:7">
@@ -10998,7 +10998,7 @@
         <v>1</v>
       </c>
       <c r="G461">
-        <v>0.5439999779440052</v>
+        <v>0.7650783312204882</v>
       </c>
     </row>
     <row r="462" spans="1:7">
@@ -11021,7 +11021,7 @@
         <v>5</v>
       </c>
       <c r="G462">
-        <v>0.2360173550580451</v>
+        <v>0.02797945203263821</v>
       </c>
     </row>
     <row r="463" spans="1:7">
@@ -11044,7 +11044,7 @@
         <v>5</v>
       </c>
       <c r="G463">
-        <v>0.5715925621207849</v>
+        <v>0.3014043390980348</v>
       </c>
     </row>
     <row r="464" spans="1:7">
@@ -11067,7 +11067,7 @@
         <v>3</v>
       </c>
       <c r="G464">
-        <v>0.261898448674198</v>
+        <v>0.3176958855658047</v>
       </c>
     </row>
     <row r="465" spans="1:7">
@@ -11090,7 +11090,7 @@
         <v>3</v>
       </c>
       <c r="G465">
-        <v>0.2195113640556061</v>
+        <v>0.2380003563932978</v>
       </c>
     </row>
     <row r="466" spans="1:7">
@@ -11113,7 +11113,7 @@
         <v>3</v>
       </c>
       <c r="G466">
-        <v>0.6331177494911424</v>
+        <v>0.5706830617353715</v>
       </c>
     </row>
     <row r="467" spans="1:7">
@@ -11136,7 +11136,7 @@
         <v>0</v>
       </c>
       <c r="G467">
-        <v>0.4795413395675203</v>
+        <v>0.853485928732721</v>
       </c>
     </row>
     <row r="468" spans="1:7">
@@ -11159,7 +11159,7 @@
         <v>0</v>
       </c>
       <c r="G468">
-        <v>0.4722763616564946</v>
+        <v>0.8491669783968616</v>
       </c>
     </row>
     <row r="469" spans="1:7">
@@ -11182,7 +11182,7 @@
         <v>5</v>
       </c>
       <c r="G469">
-        <v>0.4320211290749789</v>
+        <v>0.2312564637096431</v>
       </c>
     </row>
     <row r="470" spans="1:7">
@@ -11205,7 +11205,7 @@
         <v>4</v>
       </c>
       <c r="G470">
-        <v>0.9156153728061098</v>
+        <v>0.5799581912786809</v>
       </c>
     </row>
     <row r="471" spans="1:7">
@@ -11228,7 +11228,7 @@
         <v>2</v>
       </c>
       <c r="G471">
-        <v>0.7559718995209029</v>
+        <v>0.7650088449725019</v>
       </c>
     </row>
     <row r="472" spans="1:7">
@@ -11251,7 +11251,7 @@
         <v>2</v>
       </c>
       <c r="G472">
-        <v>0.4773710729589009</v>
+        <v>0.6067779339123859</v>
       </c>
     </row>
     <row r="473" spans="1:7">
@@ -11274,7 +11274,7 @@
         <v>1</v>
       </c>
       <c r="G473">
-        <v>0.4910219553237251</v>
+        <v>0.7429518210498668</v>
       </c>
     </row>
     <row r="474" spans="1:7">
@@ -11297,7 +11297,7 @@
         <v>4</v>
       </c>
       <c r="G474">
-        <v>0.3484310335449045</v>
+        <v>0.2438488683426262</v>
       </c>
     </row>
     <row r="475" spans="1:7">
@@ -11320,7 +11320,7 @@
         <v>0</v>
       </c>
       <c r="G475">
-        <v>0.5758188530279217</v>
+        <v>0.9258634767994663</v>
       </c>
     </row>
     <row r="476" spans="1:7">
@@ -11343,7 +11343,7 @@
         <v>0</v>
       </c>
       <c r="G476">
-        <v>0.2695806959536538</v>
+        <v>0.6423850038334326</v>
       </c>
     </row>
     <row r="477" spans="1:7">
@@ -11366,7 +11366,7 @@
         <v>3</v>
       </c>
       <c r="G477">
-        <v>0.2819200298445586</v>
+        <v>0.3456753375984429</v>
       </c>
     </row>
     <row r="478" spans="1:7">
@@ -11389,7 +11389,7 @@
         <v>4</v>
       </c>
       <c r="G478">
-        <v>0.6762615608912425</v>
+        <v>0.5012820843905066</v>
       </c>
     </row>
     <row r="479" spans="1:7">
@@ -11412,7 +11412,7 @@
         <v>4</v>
       </c>
       <c r="G479">
-        <v>0.6012081193389918</v>
+        <v>0.4671265591363963</v>
       </c>
     </row>
     <row r="480" spans="1:7">
@@ -11435,7 +11435,7 @@
         <v>0</v>
       </c>
       <c r="G480">
-        <v>0.5464148568699608</v>
+        <v>0.9072200915068738</v>
       </c>
     </row>
     <row r="481" spans="1:7">
@@ -11458,7 +11458,7 @@
         <v>4</v>
       </c>
       <c r="G481">
-        <v>0.6652466352663791</v>
+        <v>0.4966635474753013</v>
       </c>
     </row>
     <row r="482" spans="1:7">
@@ -11481,7 +11481,7 @@
         <v>3</v>
       </c>
       <c r="G482">
-        <v>0.4396516534540901</v>
+        <v>0.4813297708362262</v>
       </c>
     </row>
     <row r="483" spans="1:7">
@@ -11504,7 +11504,7 @@
         <v>3</v>
       </c>
       <c r="G483">
-        <v>0.8290640995938786</v>
+        <v>0.6780706146167373</v>
       </c>
     </row>
     <row r="484" spans="1:7">
@@ -11527,7 +11527,7 @@
         <v>5</v>
       </c>
       <c r="G484">
-        <v>0.5157492584663591</v>
+        <v>0.2765676359215429</v>
       </c>
     </row>
     <row r="485" spans="1:7">
@@ -11550,7 +11550,7 @@
         <v>0</v>
       </c>
       <c r="G485">
-        <v>0.4710962068896405</v>
+        <v>0.8479622732301967</v>
       </c>
     </row>
     <row r="486" spans="1:7">
@@ -11573,7 +11573,7 @@
         <v>0</v>
       </c>
       <c r="G486">
-        <v>0.4163464503436116</v>
+        <v>0.8118349707773724</v>
       </c>
     </row>
     <row r="487" spans="1:7">
@@ -11596,7 +11596,7 @@
         <v>4</v>
       </c>
       <c r="G487">
-        <v>0.4047036021198361</v>
+        <v>0.3362669158899729</v>
       </c>
     </row>
     <row r="488" spans="1:7">
@@ -11619,7 +11619,7 @@
         <v>5</v>
       </c>
       <c r="G488">
-        <v>0.7158276848205343</v>
+        <v>0.352964250882649</v>
       </c>
     </row>
     <row r="489" spans="1:7">
@@ -11642,7 +11642,7 @@
         <v>4</v>
       </c>
       <c r="G489">
-        <v>0.395695646221109</v>
+        <v>0.3300181763172585</v>
       </c>
     </row>
     <row r="490" spans="1:7">
@@ -11665,7 +11665,7 @@
         <v>5</v>
       </c>
       <c r="G490">
-        <v>0.4796770266642348</v>
+        <v>0.2696200672007749</v>
       </c>
     </row>
     <row r="491" spans="1:7">
@@ -11688,7 +11688,7 @@
         <v>5</v>
       </c>
       <c r="G491">
-        <v>0.4992067504402891</v>
+        <v>0.2839781140898264</v>
       </c>
     </row>
     <row r="492" spans="1:7">
@@ -11711,7 +11711,7 @@
         <v>5</v>
       </c>
       <c r="G492">
-        <v>0.6044192481730681</v>
+        <v>0.346016682161881</v>
       </c>
     </row>
     <row r="493" spans="1:7">
@@ -11734,7 +11734,7 @@
         <v>2</v>
       </c>
       <c r="G493">
-        <v>0.5289990707712156</v>
+        <v>0.6497459424410644</v>
       </c>
     </row>
     <row r="494" spans="1:7">
@@ -11757,7 +11757,7 @@
         <v>4</v>
       </c>
       <c r="G494">
-        <v>0.3768880117333277</v>
+        <v>0.2882116139072844</v>
       </c>
     </row>
     <row r="495" spans="1:7">
@@ -11780,7 +11780,7 @@
         <v>4</v>
       </c>
       <c r="G495">
-        <v>0.3439336951442158</v>
+        <v>0.2890820483465811</v>
       </c>
     </row>
     <row r="496" spans="1:7">
@@ -11803,7 +11803,7 @@
         <v>1</v>
       </c>
       <c r="G496">
-        <v>0.4839244960673041</v>
+        <v>0.7368467434654858</v>
       </c>
     </row>
     <row r="497" spans="1:7">
@@ -11826,7 +11826,7 @@
         <v>5</v>
       </c>
       <c r="G497">
-        <v>0.4220657981843978</v>
+        <v>0.2250077241369288</v>
       </c>
     </row>
     <row r="498" spans="1:7">
@@ -11849,7 +11849,7 @@
         <v>0</v>
       </c>
       <c r="G498">
-        <v>0.5609878735085195</v>
+        <v>0.9167053561966205</v>
       </c>
     </row>
     <row r="499" spans="1:7">
@@ -11872,7 +11872,7 @@
         <v>4</v>
       </c>
       <c r="G499">
-        <v>0.5730838162001197</v>
+        <v>0.4247364815843645</v>
       </c>
     </row>
     <row r="500" spans="1:7">
@@ -11895,7 +11895,7 @@
         <v>1</v>
       </c>
       <c r="G500">
-        <v>0.7663718269656241</v>
+        <v>0.8915629302256894</v>
       </c>
     </row>
     <row r="501" spans="1:7">
@@ -11918,7 +11918,7 @@
         <v>4</v>
       </c>
       <c r="G501">
-        <v>0.4323548659300354</v>
+        <v>0.3541765670458812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>